<commit_message>
Promo changes and new org test data changes
</commit_message>
<xml_diff>
--- a/TestData/AdminConsole/Promo/promo_test_data.xlsx
+++ b/TestData/AdminConsole/Promo/promo_test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Ginesys Zwing\Ginesys_Zwing_Automation\TestData\AdminConsole\Promo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\AdminConsole\Promo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1085,8 +1085,8 @@
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A61">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="L43">
+      <selection activeCell="P52" sqref="P52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -4525,8 +4525,8 @@
       <c r="Q49" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R49" s="1">
-        <v>1</v>
+      <c r="R49" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="S49" s="1" t="s">
         <v>35</v>

</xml_diff>